<commit_message>
fixed bug in leakage model
Signed-off-by: Craig <cbradsha@purdue.edu>
</commit_message>
<xml_diff>
--- a/master_sens_studies/ecc_g_1_11/data_log_ecc_g.xlsx
+++ b/master_sens_studies/ecc_g_1_11/data_log_ecc_g.xlsx
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AZ38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="AO3" sqref="AO3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>